<commit_message>
Poultry paramaters and scenario files updated
</commit_message>
<xml_diff>
--- a/Ethiopia Workspace/Code and Control Files/AHLE scenario parameters POULTRY.xlsx
+++ b/Ethiopia Workspace/Code and Control Files/AHLE scenario parameters POULTRY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gemmachaters/Dropbox/Mac/Documents/GitHub/GBADsLiverpool/Ethiopia Workspace/Code and Control Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1CD0848-ADFB-D84B-97D2-8BE2EEFB9925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FD179C-B8A1-A148-B67A-258EAA6FE026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="640" windowWidth="27300" windowHeight="16140" xr2:uid="{7B09E95E-6D5F-461A-A5DC-5B71F2D22658}"/>
+    <workbookView xWindow="0" yWindow="640" windowWidth="10200" windowHeight="16140" xr2:uid="{7B09E95E-6D5F-461A-A5DC-5B71F2D22658}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="157">
   <si>
     <t># Initial population</t>
   </si>
@@ -478,18 +478,6 @@
     <t># offtake rate female</t>
   </si>
   <si>
-    <t>0.574/12</t>
-  </si>
-  <si>
-    <t>rpert(10000, 12, 25, 18.5)</t>
-  </si>
-  <si>
-    <t>rpert(10000, 13, 22, 17.5)</t>
-  </si>
-  <si>
-    <t>rpert(10000, 15, 22, 18.5)</t>
-  </si>
-  <si>
     <t># Neonatal female (0-8weeks)</t>
   </si>
   <si>
@@ -569,6 +557,24 @@
   </si>
   <si>
     <t>rpert(10000, 2.97, 5, 4)</t>
+  </si>
+  <si>
+    <t>rpert(10000, 0.15, 0.22, 0.185)</t>
+  </si>
+  <si>
+    <t>rpert(10000, 0.13, 0.22, 0.175)</t>
+  </si>
+  <si>
+    <t>0.574/2</t>
+  </si>
+  <si>
+    <t>rpert(10000, 0.12/4, 0.25/4, 0.185/4)</t>
+  </si>
+  <si>
+    <t>rpert(10000, 0.987, 1.3, 1.15)</t>
+  </si>
+  <si>
+    <t>rpert(10000, 0.59, 0.8, 0.7)</t>
   </si>
 </sst>
 </file>
@@ -1196,16 +1202,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDE79AB-593E-49D8-BC0E-644D5608E970}">
   <dimension ref="A1:XFD129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="63" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="63" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B21" sqref="B21"/>
+      <selection pane="topRight" activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="40.6640625" style="13" customWidth="1"/>
     <col min="2" max="2" width="80.5" customWidth="1"/>
-    <col min="3" max="5" width="39.6640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="33" customWidth="1"/>
+    <col min="4" max="5" width="39.6640625" style="33" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="39.6640625" style="17" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="41.6640625" style="21" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.6640625" style="33" customWidth="1"/>
@@ -1478,17 +1485,10 @@
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="3">
-        <v>56992987</v>
-      </c>
-      <c r="F4" s="17">
-        <v>56992987</v>
-      </c>
+      <c r="F4" s="17"/>
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
-      <c r="I4" s="21">
-        <v>56992987</v>
-      </c>
+      <c r="I4" s="21"/>
       <c r="J4" s="21"/>
       <c r="K4" s="21"/>
       <c r="AV4" s="5"/>
@@ -1504,45 +1504,21 @@
       <c r="A5" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="C5" s="33">
-        <f>C4*0.89</f>
-        <v>50723758.43</v>
-      </c>
-      <c r="F5" s="17">
-        <f>F4*0.89</f>
-        <v>50723758.43</v>
-      </c>
-      <c r="I5" s="21">
-        <f>I4*0.055</f>
-        <v>3134614.2850000001</v>
-      </c>
     </row>
     <row r="6" spans="1:871" s="59" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="59" t="s">
         <v>121</v>
       </c>
-      <c r="C6" s="59">
-        <f>C5*0.78</f>
-        <v>39564531.575400002</v>
-      </c>
-      <c r="F6" s="59">
-        <f>F5*0.22</f>
-        <v>11159226.854599999</v>
-      </c>
-      <c r="I6" s="59">
-        <f>I5*1</f>
-        <v>3134614.2850000001</v>
-      </c>
     </row>
     <row r="7" spans="1:871" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C7" s="60">
-        <v>6500452.5378382206</v>
+        <v>6500452</v>
       </c>
       <c r="D7" s="60">
         <v>6500452.5378382206</v>
@@ -1613,7 +1589,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="60">
-        <v>6500452.5378382206</v>
+        <v>6500452</v>
       </c>
       <c r="D8" s="60">
         <v>6500452.5378382206</v>
@@ -1684,7 +1660,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="60">
-        <v>4494530.786965441</v>
+        <v>4494530</v>
       </c>
       <c r="D9" s="60">
         <v>4494530.786965441</v>
@@ -2559,7 +2535,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="60">
-        <v>2271004.1124279601</v>
+        <v>2271004</v>
       </c>
       <c r="D10" s="60">
         <v>2271004.1124279601</v>
@@ -3434,7 +3410,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="60">
-        <v>15370820.517042901</v>
+        <v>15370820</v>
       </c>
       <c r="D11" s="60">
         <v>15370820.517042901</v>
@@ -4309,7 +4285,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="60">
-        <v>4431227.5364448</v>
+        <v>4431227</v>
       </c>
       <c r="D12" s="60">
         <v>4431227.5364448</v>
@@ -7037,10 +7013,10 @@
     </row>
     <row r="19" spans="1:871" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="68" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C19" s="63">
-        <v>0.88</v>
+        <v>0.8</v>
       </c>
       <c r="D19" s="63">
         <v>0.88</v>
@@ -7079,32 +7055,32 @@
       <c r="A20" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C20" s="63" t="s">
-        <v>141</v>
+      <c r="C20" s="63">
+        <v>0.2</v>
       </c>
       <c r="D20" s="63" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E20" s="63" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="I20" s="21" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="K20" s="21" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="O20" s="39"/>
       <c r="T20" s="47"/>
@@ -7938,7 +7914,7 @@
     </row>
     <row r="21" spans="1:871" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C21" s="63">
         <v>0.51</v>
@@ -8799,7 +8775,7 @@
     </row>
     <row r="22" spans="1:871" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C22" s="63">
         <v>0.23</v>
@@ -9660,7 +9636,7 @@
     </row>
     <row r="23" spans="1:871" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C23" s="63">
         <v>0.2</v>
@@ -11377,34 +11353,34 @@
     </row>
     <row r="25" spans="1:871" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="AV25" s="5"/>
       <c r="AW25" s="5"/>
@@ -16779,8 +16755,9 @@
       <c r="B37" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="62" t="s">
-        <v>124</v>
+      <c r="C37" s="62">
+        <f>0.574/2</f>
+        <v>0.28699999999999998</v>
       </c>
       <c r="D37" s="65">
         <v>0</v>
@@ -16789,7 +16766,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="55" t="s">
-        <v>124</v>
+        <v>153</v>
       </c>
       <c r="G37" s="66">
         <v>0</v>
@@ -16798,7 +16775,7 @@
         <v>0</v>
       </c>
       <c r="I37" s="58" t="s">
-        <v>124</v>
+        <v>153</v>
       </c>
       <c r="J37" s="67">
         <v>0</v>
@@ -17676,7 +17653,7 @@
         <v>14</v>
       </c>
       <c r="C38" s="62" t="s">
-        <v>125</v>
+        <v>154</v>
       </c>
       <c r="D38" s="65">
         <v>0</v>
@@ -17685,7 +17662,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="55" t="s">
-        <v>125</v>
+        <v>154</v>
       </c>
       <c r="G38" s="66">
         <v>0</v>
@@ -17694,7 +17671,7 @@
         <v>0</v>
       </c>
       <c r="I38" s="58" t="s">
-        <v>125</v>
+        <v>154</v>
       </c>
       <c r="J38" s="67">
         <v>0</v>
@@ -18580,7 +18557,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="55" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="G39" s="66">
         <v>0</v>
@@ -18589,7 +18566,7 @@
         <v>0</v>
       </c>
       <c r="I39" s="58" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="J39" s="67">
         <v>0</v>
@@ -19466,7 +19443,7 @@
         <v>16</v>
       </c>
       <c r="C40" s="62" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
       <c r="D40" s="65">
         <v>0</v>
@@ -19475,7 +19452,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="55" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
       <c r="G40" s="66">
         <v>0</v>
@@ -19484,7 +19461,7 @@
         <v>0</v>
       </c>
       <c r="I40" s="58" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
       <c r="J40" s="67">
         <v>0</v>
@@ -20432,7 +20409,7 @@
         <v>67</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C43" s="33">
         <f>1/46</f>
@@ -21294,17 +21271,14 @@
       <c r="AGK43" s="3"/>
       <c r="AGL43" s="3"/>
       <c r="AGM43" s="3"/>
-      <c r="XFD43" s="33">
-        <f>1/106</f>
-        <v>9.433962264150943E-3</v>
-      </c>
+      <c r="XFD43" s="33"/>
     </row>
     <row r="44" spans="1:871 16384:16384" x14ac:dyDescent="0.2">
       <c r="A44" s="16" t="s">
         <v>68</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C44" s="33">
         <f>1/43</f>
@@ -22166,10 +22140,7 @@
       <c r="AGK44" s="3"/>
       <c r="AGL44" s="3"/>
       <c r="AGM44" s="3"/>
-      <c r="XFD44" s="33">
-        <f>1/106</f>
-        <v>9.433962264150943E-3</v>
-      </c>
+      <c r="XFD44" s="33"/>
     </row>
     <row r="45" spans="1:871 16384:16384" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
@@ -22233,31 +22204,31 @@
         <v>20</v>
       </c>
       <c r="C48" s="33" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D48" s="33" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E48" s="33" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F48" s="17" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G48" s="17" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H48" s="17" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="I48" s="21" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="J48" s="21" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="K48" s="21" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="AV48" s="5"/>
       <c r="AW48" s="5"/>
@@ -23092,31 +23063,31 @@
         <v>21</v>
       </c>
       <c r="C49" s="33" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D49" s="33" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E49" s="33" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F49" s="17" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G49" s="17" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H49" s="17" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="I49" s="21" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="J49" s="21" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="K49" s="21" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="AV49" s="5"/>
       <c r="AW49" s="5"/>
@@ -23951,31 +23922,31 @@
         <v>22</v>
       </c>
       <c r="C50" s="33" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="D50" s="33" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E50" s="33" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F50" s="17" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="G50" s="17" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="H50" s="17" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="I50" s="21" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="J50" s="21" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="K50" s="21" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="AV50" s="5"/>
       <c r="AW50" s="5"/>
@@ -24810,31 +24781,31 @@
         <v>23</v>
       </c>
       <c r="C51" s="64" t="s">
+        <v>156</v>
+      </c>
+      <c r="D51" s="64" t="s">
+        <v>128</v>
+      </c>
+      <c r="E51" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="F51" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="D51" s="64" t="s">
+      <c r="G51" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="E51" s="33" t="s">
+      <c r="H51" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="F51" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="G51" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="H51" s="17" t="s">
-        <v>136</v>
-      </c>
       <c r="I51" s="21" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="J51" s="21" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="K51" s="21" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="AV51" s="5"/>
       <c r="AW51" s="5"/>
@@ -25669,31 +25640,31 @@
         <v>24</v>
       </c>
       <c r="C52" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="D52" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="E52" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="F52" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="D52" s="33" t="s">
+      <c r="G52" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="E52" s="33" t="s">
+      <c r="H52" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="F52" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="G52" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="H52" s="17" t="s">
-        <v>137</v>
-      </c>
       <c r="I52" s="21" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J52" s="21" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K52" s="21" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="AV52" s="5"/>
       <c r="AW52" s="5"/>
@@ -26528,31 +26499,31 @@
         <v>24</v>
       </c>
       <c r="C53" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="D53" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="E53" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="F53" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="D53" s="33" t="s">
+      <c r="G53" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="E53" s="33" t="s">
+      <c r="H53" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="F53" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="G53" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="H53" s="17" t="s">
-        <v>138</v>
-      </c>
       <c r="I53" s="21" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="J53" s="21" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K53" s="21" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="AV53" s="5"/>
       <c r="AW53" s="5"/>
@@ -28335,7 +28306,7 @@
         <v>29</v>
       </c>
       <c r="C60" s="33">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D60" s="33">
         <v>0</v>
@@ -29198,7 +29169,7 @@
         <v>30</v>
       </c>
       <c r="C61" s="33">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D61" s="33">
         <v>0</v>
@@ -30062,7 +30033,7 @@
         <v>31</v>
       </c>
       <c r="C62" s="33">
-        <v>0</v>
+        <v>92.88</v>
       </c>
       <c r="D62" s="33">
         <v>0</v>
@@ -30926,7 +30897,7 @@
         <v>32</v>
       </c>
       <c r="C63" s="33">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D63" s="33">
         <v>0</v>
@@ -31790,7 +31761,7 @@
         <v>33</v>
       </c>
       <c r="C64" s="33">
-        <v>92.88</v>
+        <v>20</v>
       </c>
       <c r="D64" s="33">
         <v>92.88</v>
@@ -33544,7 +33515,7 @@
     </row>
     <row r="68" spans="1:871" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F68" s="17"/>
       <c r="G68" s="17"/>
@@ -33563,13 +33534,12 @@
     </row>
     <row r="69" spans="1:871" x14ac:dyDescent="0.2">
       <c r="A69" s="16" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B69" s="16" t="s">
         <v>35</v>
       </c>
       <c r="C69" s="33">
-        <f>(1.66/6)*4.25</f>
         <v>1.1758333333333333</v>
       </c>
       <c r="D69" s="33">
@@ -34431,13 +34401,12 @@
     </row>
     <row r="70" spans="1:871" x14ac:dyDescent="0.2">
       <c r="A70" s="16" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B70" s="16" t="s">
         <v>35</v>
       </c>
       <c r="C70" s="33">
-        <f>(1.66/6)*4.25</f>
         <v>1.1758333333333333</v>
       </c>
       <c r="D70" s="33">
@@ -35299,13 +35268,12 @@
     </row>
     <row r="71" spans="1:871" x14ac:dyDescent="0.2">
       <c r="A71" s="16" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B71" s="16" t="s">
         <v>36</v>
       </c>
       <c r="C71" s="33">
-        <f>(8.53/15)*4.25</f>
         <v>2.4168333333333334</v>
       </c>
       <c r="D71" s="33">
@@ -36167,13 +36135,12 @@
     </row>
     <row r="72" spans="1:871" x14ac:dyDescent="0.2">
       <c r="A72" s="16" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B72" s="16" t="s">
         <v>36</v>
       </c>
       <c r="C72" s="33">
-        <f>(8.3/15)*4.25</f>
         <v>2.3516666666666666</v>
       </c>
       <c r="D72" s="33">
@@ -37035,13 +37002,12 @@
     </row>
     <row r="73" spans="1:871" x14ac:dyDescent="0.2">
       <c r="A73" s="16" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B73" s="16" t="s">
         <v>37</v>
       </c>
       <c r="C73" s="33">
-        <f>36/12</f>
         <v>3</v>
       </c>
       <c r="D73" s="33">
@@ -37903,13 +37869,12 @@
     </row>
     <row r="74" spans="1:871" x14ac:dyDescent="0.2">
       <c r="A74" s="16" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B74" s="16" t="s">
         <v>37</v>
       </c>
       <c r="C74" s="33">
-        <f>45/12</f>
         <v>3.75</v>
       </c>
       <c r="D74" s="33">
@@ -42527,13 +42492,13 @@
         <v>0</v>
       </c>
       <c r="I95" s="21" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J95" s="21" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="K95" s="21" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="AV95" s="5"/>
       <c r="AW95" s="5"/>

</xml_diff>

<commit_message>
most recent poultry scenario
</commit_message>
<xml_diff>
--- a/Ethiopia Workspace/Code and Control Files/AHLE scenario parameters POULTRY.xlsx
+++ b/Ethiopia Workspace/Code and Control Files/AHLE scenario parameters POULTRY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gemmachaters/Dropbox/Mac/Documents/GitHub/GBADsLiverpool/Ethiopia Workspace/Code and Control Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3535CF4-95B2-6143-987B-CE55F4FF7F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13E83B4-5304-5545-8147-32EAB1B87822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="520" yWindow="1160" windowWidth="28800" windowHeight="16180" xr2:uid="{7B09E95E-6D5F-461A-A5DC-5B71F2D22658}"/>
   </bookViews>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="163">
   <si>
     <t># Initial population</t>
   </si>
@@ -554,9 +554,6 @@
   </si>
   <si>
     <t>rpert(10000, 0.13, 0.22, 0.175)</t>
-  </si>
-  <si>
-    <t>0.574/2</t>
   </si>
   <si>
     <t>rpert(10000, 0.12/4, 0.25/4, 0.185/4)</t>
@@ -1239,10 +1236,10 @@
   <dimension ref="A1:XFD129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F38" sqref="F38"/>
+      <selection pane="bottomRight" activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7100,7 +7097,7 @@
         <v>134</v>
       </c>
       <c r="E20" s="39" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F20" s="17" t="s">
         <v>134</v>
@@ -7109,7 +7106,7 @@
         <v>134</v>
       </c>
       <c r="H20" s="47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I20" s="21" t="s">
         <v>135</v>
@@ -7118,7 +7115,7 @@
         <v>135</v>
       </c>
       <c r="K20" s="71" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O20" s="39"/>
       <c r="T20" s="47"/>
@@ -8813,7 +8810,7 @@
     </row>
     <row r="22" spans="1:871" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C22" s="63">
         <v>0.23</v>
@@ -16803,8 +16800,9 @@
       <c r="E37" s="65">
         <v>0</v>
       </c>
-      <c r="F37" s="55" t="s">
-        <v>150</v>
+      <c r="F37" s="55">
+        <f>0.574/2</f>
+        <v>0.28699999999999998</v>
       </c>
       <c r="G37" s="66">
         <v>0</v>
@@ -16812,8 +16810,9 @@
       <c r="H37" s="66">
         <v>0</v>
       </c>
-      <c r="I37" s="58" t="s">
-        <v>150</v>
+      <c r="I37" s="58">
+        <f>0.574/2</f>
+        <v>0.28699999999999998</v>
       </c>
       <c r="J37" s="67">
         <v>0</v>
@@ -17691,7 +17690,7 @@
         <v>14</v>
       </c>
       <c r="C38" s="62" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D38" s="65">
         <v>0</v>
@@ -17700,7 +17699,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="55" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G38" s="66">
         <v>0</v>
@@ -17709,7 +17708,7 @@
         <v>0</v>
       </c>
       <c r="I38" s="58" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J38" s="67">
         <v>0</v>
@@ -22248,7 +22247,7 @@
         <v>127</v>
       </c>
       <c r="E48" s="39" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F48" s="17" t="s">
         <v>127</v>
@@ -23107,7 +23106,7 @@
         <v>127</v>
       </c>
       <c r="E49" s="39" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F49" s="17" t="s">
         <v>127</v>
@@ -23960,13 +23959,13 @@
         <v>22</v>
       </c>
       <c r="C50" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D50" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E50" s="39" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F50" s="17" t="s">
         <v>129</v>
@@ -24819,13 +24818,13 @@
         <v>23</v>
       </c>
       <c r="C51" s="64" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D51" s="64" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E51" s="70" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F51" s="17" t="s">
         <v>130</v>
@@ -25684,7 +25683,7 @@
         <v>128</v>
       </c>
       <c r="E52" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F52" s="17" t="s">
         <v>131</v>
@@ -26537,13 +26536,13 @@
         <v>24</v>
       </c>
       <c r="C53" s="69" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D53" s="69" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E53" s="39" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F53" s="17" t="s">
         <v>132</v>

</xml_diff>

<commit_message>
new small ruminant results
</commit_message>
<xml_diff>
--- a/Ethiopia Workspace/Code and Control Files/AHLE scenario parameters POULTRY.xlsx
+++ b/Ethiopia Workspace/Code and Control Files/AHLE scenario parameters POULTRY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gemmachaters/Dropbox/Mac/Documents/GitHub/GBADsLiverpool/Ethiopia Workspace/Code and Control Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F61D9A-2728-3141-9BF4-EEF47B1B6E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9664C97E-B51A-A047-B85F-35A52716102C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="1160" windowWidth="28800" windowHeight="14880" xr2:uid="{7B09E95E-6D5F-461A-A5DC-5B71F2D22658}"/>
+    <workbookView xWindow="0" yWindow="1160" windowWidth="28800" windowHeight="14880" activeTab="1" xr2:uid="{7B09E95E-6D5F-461A-A5DC-5B71F2D22658}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="197">
   <si>
     <t># Initial population</t>
   </si>
@@ -678,13 +678,31 @@
   <si>
     <t xml:space="preserve"> mort zero</t>
   </si>
+  <si>
+    <t>vill ind current</t>
+  </si>
+  <si>
+    <t>vil ind juv mort zero</t>
+  </si>
+  <si>
+    <t>vil ind juv ideal</t>
+  </si>
+  <si>
+    <t>AHLE</t>
+  </si>
+  <si>
+    <t>Juv</t>
+  </si>
+  <si>
+    <t>prod AHLE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -855,7 +873,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -899,7 +917,7 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -924,7 +942,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -934,27 +952,28 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1271,11 +1290,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDE79AB-593E-49D8-BC0E-644D5608E970}">
   <dimension ref="A1:XCJ213"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="20" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K18" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="89" zoomScaleNormal="20" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P11" sqref="P11"/>
+      <selection pane="bottomRight" activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1286,6 +1305,7 @@
     <col min="4" max="5" width="39.6640625" style="20" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="39.6640625" style="12" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="41.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="35" customWidth="1"/>
     <col min="17" max="17" width="26" customWidth="1"/>
   </cols>
@@ -1540,6 +1560,12 @@
     <row r="6" spans="1:799" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="42" t="s">
         <v>118</v>
+      </c>
+      <c r="C6" s="55"/>
+      <c r="L6" s="55"/>
+      <c r="U6" s="42">
+        <f>SUM(U7:U12)</f>
+        <v>3129285.4407155002</v>
       </c>
     </row>
     <row r="7" spans="1:799" x14ac:dyDescent="0.2">
@@ -48127,16 +48153,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3D08064-68C3-4BB0-A64D-3A606C4D4B6B}">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" zoomScale="138" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="B23" zoomScale="138" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38:F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.33203125" customWidth="1"/>
     <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.83203125" customWidth="1"/>
@@ -48309,6 +48336,69 @@
         <v>0</v>
       </c>
     </row>
+    <row r="30" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E30" t="s">
+        <v>191</v>
+      </c>
+      <c r="F30" s="54">
+        <v>9154907178.8783302</v>
+      </c>
+    </row>
+    <row r="31" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E31" t="s">
+        <v>192</v>
+      </c>
+      <c r="F31" s="54">
+        <v>10954558648.7402</v>
+      </c>
+    </row>
+    <row r="32" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E32" t="s">
+        <v>193</v>
+      </c>
+      <c r="F32" s="54">
+        <v>12965788832.187099</v>
+      </c>
+    </row>
+    <row r="33" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F33" t="s">
+        <v>195</v>
+      </c>
+      <c r="G33" t="s">
+        <v>194</v>
+      </c>
+      <c r="H33">
+        <f>F32-F30</f>
+        <v>3810881653.3087692</v>
+      </c>
+    </row>
+    <row r="34" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F34" t="s">
+        <v>195</v>
+      </c>
+      <c r="G34" t="s">
+        <v>181</v>
+      </c>
+      <c r="H34">
+        <f>F31-F30</f>
+        <v>1799651469.8618698</v>
+      </c>
+    </row>
+    <row r="35" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="G35" t="s">
+        <v>196</v>
+      </c>
+      <c r="H35">
+        <f>H33-H34</f>
+        <v>2011230183.4468994</v>
+      </c>
+    </row>
+    <row r="38" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F38" s="54"/>
+    </row>
+    <row r="39" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F39" s="54"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>